<commit_message>
new FLOSPA code to generate all possible cases.
</commit_message>
<xml_diff>
--- a/Previous Work/genmix.xlsx
+++ b/Previous Work/genmix.xlsx
@@ -3095,11 +3095,11 @@
   </sheetPr>
   <dimension ref="A2:G1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A528" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I208" activeCellId="0" sqref="I208"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A862" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="31.015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="59.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.07"/>
@@ -3108,6 +3108,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.09"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>